<commit_message>
Removed ATAPS mapping. Not relevant for version 2.
</commit_message>
<xml_diff>
--- a/doc/_data/_orig/pmhc-upload.xlsx
+++ b/doc/_data/_orig/pmhc-upload.xlsx
@@ -5,12 +5,12 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jenni/Work/git/PMHC/spec/data/_orig/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/russellj/stratdat/pmhc/spec/data/_orig/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CAA1B3C-1363-664E-849A-8C351EDAE5D9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5837FB5A-3B28-6C46-BE55-CE1DE1266331}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38860" yWindow="3780" windowWidth="32120" windowHeight="16060" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="28340" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="9" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="185">
   <si>
     <t>organisation_path</t>
   </si>
@@ -563,18 +563,9 @@
     <t>organisation_start_date</t>
   </si>
   <si>
-    <t>01072016</t>
-  </si>
-  <si>
     <t>organisation_end_date</t>
   </si>
   <si>
-    <t>organisation_omsss_email</t>
-  </si>
-  <si>
-    <t>org1@mail.example.com</t>
-  </si>
-  <si>
     <t>key</t>
   </si>
   <si>
@@ -591,6 +582,12 @@
   </si>
   <si>
     <t>continuity_of_support</t>
+  </si>
+  <si>
+    <t>01072014</t>
+  </si>
+  <si>
+    <t>09099999</t>
   </si>
 </sst>
 </file>
@@ -646,26 +643,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="5" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -969,30 +963,30 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="AE22" sqref="AE22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B2" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -1164,7 +1158,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AC5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AC5" sqref="AC5"/>
     </sheetView>
   </sheetViews>
@@ -1253,7 +1247,7 @@
         <v>43</v>
       </c>
       <c r="AB1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="AC1" t="s">
         <v>44</v>
@@ -2272,9 +2266,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:BD3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2794,7 +2786,7 @@
         <v>3</v>
       </c>
       <c r="BB3">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="BC3">
         <v>5</v>
@@ -2950,10 +2942,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2963,10 +2955,10 @@
     <col min="3" max="3" width="25.6640625" customWidth="1"/>
     <col min="4" max="4" width="21.6640625" customWidth="1"/>
     <col min="5" max="5" width="20.5" customWidth="1"/>
-    <col min="8" max="10" width="10.83203125" style="2"/>
+    <col min="8" max="9" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2992,16 +2984,13 @@
         <v>175</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="K1" t="s">
+        <v>176</v>
+      </c>
+      <c r="J1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -3021,16 +3010,13 @@
         <v>1</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>179</v>
+        <v>183</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>184</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="J2" r:id="rId1" xr:uid="{7B3AA911-53A5-3445-88E8-2DB7B9629137}"/>
-  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>